<commit_message>
Mapping de la partie corps entre modèle métier / CDA / FHIR (#90)
* Ajout des ressources CDA Corps

* Correction de l'erreur du type IVL_INT

* Delete input/fsh/MappingML_CDA_FHIR_Corps directory

* Stop tracking local working repositories

* Mapping entre ML/CDA/FHIR de la partie corps

* Création de nx mappings

* MAJ mapping suite review de NRISS

* MAJ mapping suite review de NRISS

* MAJ modèle logique corps

* MAJ de la requete sql pour récupération des mappings de l'entete

* Création de nouveaux mapping pour le corps

* Mapping de la partie corps entre ML/CDA/FHIR

* MAJ mapping corps

* Mise à jour du mapping et correction des erreurs liées dans le ML et ressources FHIR

* Correction erreurs suite review NRISS

* Mise à jour mapping de la partie corps

* Mise à jour mapping corps ffb875cd77251bfff085def5561207076a91ad90
</commit_message>
<xml_diff>
--- a/main/ig/StructureDefinition-fr-diagnostic-report-document.xlsx
+++ b/main/ig/StructureDefinition-fr-diagnostic-report-document.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2026-01-28T14:36:08+00:00</t>
+    <t>2026-02-05T08:09:31+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -620,7 +620,7 @@
 </t>
   </si>
   <si>
-    <t>Type de résultat. Codee n LOINC.</t>
+    <t>Type de résultat</t>
   </si>
   <si>
     <t>A code or name that describes this diagnostic report.</t>

</xml_diff>